<commit_message>
updating graphs and imgs
</commit_message>
<xml_diff>
--- a/ipmt/test/search-cpm/search1.xlsx
+++ b/ipmt/test/search-cpm/search1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cavalcanti/Documents/git/ufpe/string-processing/ipmt/test/search/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cavalcanti/Documents/git/ufpe/string-processing/ipmt/test/search-cpm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B41430E-983F-834C-9964-464D3188217E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6D1786-97F0-684D-B82A-D2E791E540F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t>MEAN</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>1MB</t>
-  </si>
-  <si>
-    <t>5MB</t>
   </si>
 </sst>
 </file>
@@ -194,7 +191,7 @@
                 <a:uFillTx/>
                 <a:latin typeface="Calibri"/>
               </a:rPr>
-              <a:t>Tempo Médio de 10 Buscas do Padrão YRRCEDAQEK </a:t>
+              <a:t>Tempo Médio de 5 Buscas do Padrão YRRCEDAQEK </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="pt-BR" sz="1000" b="0">
@@ -355,7 +352,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="1"/>
                   <c:pt idx="0">
-                    <c:v>1.9465068427541915E-3</c:v>
+                    <c:v>1.341640786499874E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -367,7 +364,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="1"/>
                   <c:pt idx="0">
-                    <c:v>1.9465068427541915E-3</c:v>
+                    <c:v>1.341640786499874E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -392,7 +389,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.4300000000000002E-2</c:v>
+                  <c:v>3.4000000000000002E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -520,7 +517,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="1"/>
                   <c:pt idx="0">
-                    <c:v>5.0826502273256359E-3</c:v>
+                    <c:v>5.9413803110052012E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -532,7 +529,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="1"/>
                   <c:pt idx="0">
-                    <c:v>5.0826502273256359E-3</c:v>
+                    <c:v>5.9413803110052012E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -557,7 +554,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4.0499999999999994E-2</c:v>
+                  <c:v>2.9599999999999998E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -685,7 +682,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="1"/>
                   <c:pt idx="0">
-                    <c:v>1.1585910984179604E-2</c:v>
+                    <c:v>1.5165750888103116E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -697,7 +694,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="1"/>
                   <c:pt idx="0">
-                    <c:v>1.1585910984179604E-2</c:v>
+                    <c:v>1.5165750888103116E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -722,7 +719,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.30230000000000001</c:v>
+                  <c:v>0.29159999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -730,171 +727,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-BFED-8542-87C9-948CD8008F14}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$E$5:$E$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>5MB</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="FFC000"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="7.6980579674115007E-2"/>
-                  <c:y val="4.9142689897968612E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="outEnd"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:separator>; </c:separator>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-07FA-2743-8E1C-CF871E0CCCF1}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
-                  <a:lnSpc>
-                    <a:spcPct val="100000"/>
-                  </a:lnSpc>
-                  <a:spcBef>
-                    <a:spcPts val="0"/>
-                  </a:spcBef>
-                  <a:spcAft>
-                    <a:spcPts val="0"/>
-                  </a:spcAft>
-                  <a:tabLst/>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="pt-BR"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:separator>; </c:separator>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                  <a:prstGeom prst="rect">
-                    <a:avLst/>
-                  </a:prstGeom>
-                </c15:spPr>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>Sheet1!$G$5</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="1"/>
-                  <c:pt idx="0">
-                    <c:v>0.1554542090491971</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>Sheet1!$G$5</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="1"/>
-                  <c:pt idx="0">
-                    <c:v>0.1554542090491971</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:ln w="6345" cap="flat">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-                <a:round/>
-              </a:ln>
-            </c:spPr>
-          </c:errBars>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$F$5:$F$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1.4357</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-BFED-8542-87C9-948CD8008F14}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -916,7 +748,7 @@
         <c:axId val="895818575"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.8"/>
+          <c:max val="0.35000000000000003"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1422,8 +1254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1443,9 +1275,6 @@
       <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
       <c r="F1" t="s">
         <v>0</v>
       </c>
@@ -1458,203 +1287,141 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1">
-        <v>1.4999999999999999E-2</v>
+        <v>2E-3</v>
       </c>
-      <c r="B2" s="1">
-        <v>5.2999999999999999E-2</v>
+      <c r="B2">
+        <v>0.04</v>
       </c>
       <c r="C2" s="1">
-        <v>0.308</v>
+        <v>0.29099999999999998</v>
       </c>
-      <c r="D2" s="1">
-        <v>1.37</v>
-      </c>
+      <c r="D2" s="1"/>
       <c r="E2" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="2">
         <f>AVERAGE(A2:A1001)</f>
-        <v>1.4300000000000002E-2</v>
+        <v>3.4000000000000002E-3</v>
       </c>
       <c r="G2" s="3">
         <f>_xlfn.STDEV.S(A1:A1000)</f>
-        <v>1.9465068427541915E-3</v>
+        <v>1.341640786499874E-3</v>
       </c>
       <c r="H2" s="2">
         <f>MEDIAN(A2:A1001)</f>
-        <v>1.4499999999999999E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1">
-        <v>1.2999999999999999E-2</v>
+        <v>2E-3</v>
       </c>
-      <c r="B3" s="1">
-        <v>4.3999999999999997E-2</v>
+      <c r="B3">
+        <v>2.7E-2</v>
       </c>
       <c r="C3" s="1">
-        <v>0.28799999999999998</v>
+        <v>0.29199999999999998</v>
       </c>
-      <c r="D3" s="1">
-        <v>1.278</v>
-      </c>
+      <c r="D3" s="1"/>
       <c r="E3" t="s">
         <v>4</v>
       </c>
       <c r="F3" s="3">
         <f>AVERAGE(B2:B1001)</f>
-        <v>4.0499999999999994E-2</v>
+        <v>2.9599999999999998E-2</v>
       </c>
       <c r="G3" s="3">
         <f>_xlfn.STDEV.S(B2:B1001)</f>
-        <v>5.0826502273256359E-3</v>
+        <v>5.9413803110052012E-3</v>
       </c>
       <c r="H3" s="3">
         <f>MEDIAN(B2:B1001)</f>
-        <v>3.9E-2</v>
+        <v>2.7E-2</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1">
-        <v>1.4E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
-      <c r="B4" s="1">
-        <v>3.6999999999999998E-2</v>
+      <c r="B4">
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="C4" s="1">
-        <v>0.32900000000000001</v>
+        <v>0.28999999999999998</v>
       </c>
-      <c r="D4" s="1">
-        <v>1.2769999999999999</v>
-      </c>
+      <c r="D4" s="1"/>
       <c r="E4" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="3">
         <f>AVERAGE(C2:C1001)</f>
-        <v>0.30230000000000001</v>
+        <v>0.29159999999999997</v>
       </c>
       <c r="G4" s="3">
         <f>_xlfn.STDEV.S(C2:C1001)</f>
-        <v>1.1585910984179604E-2</v>
+        <v>1.5165750888103116E-3</v>
       </c>
       <c r="H4" s="3">
         <f>MEDIAN(C2:C1001)</f>
-        <v>0.30099999999999999</v>
+        <v>0.29099999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1">
-        <v>1.2E-2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
-      <c r="B5" s="1">
-        <v>3.7999999999999999E-2</v>
+      <c r="B5">
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="C5" s="1">
-        <v>0.30299999999999999</v>
+        <v>0.29399999999999998</v>
       </c>
-      <c r="D5" s="1">
-        <v>1.3440000000000001</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="3">
-        <f>AVERAGE(D2:D1001)</f>
-        <v>1.4357</v>
-      </c>
-      <c r="G5" s="3">
-        <f>_xlfn.STDEV.S(D2:D1001)</f>
-        <v>0.1554542090491971</v>
-      </c>
-      <c r="H5" s="3">
-        <f>MEDIAN(D2:D1001)</f>
-        <v>1.4145000000000001</v>
-      </c>
+      <c r="D5" s="1"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1">
-        <v>1.0999999999999999E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
-      <c r="B6" s="1">
-        <v>0.04</v>
+      <c r="B6">
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="C6" s="1">
-        <v>0.29899999999999999</v>
+        <v>0.29099999999999998</v>
       </c>
-      <c r="D6" s="1">
-        <v>1.2789999999999999</v>
-      </c>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="1">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="B7" s="1">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0.29799999999999999</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1.4590000000000001</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="1">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="B8" s="1">
-        <v>4.2000000000000003E-2</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0.29199999999999998</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1.738</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="1">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="B9" s="1">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0.29299999999999998</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1.532</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="1">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="B10" s="1">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0.307</v>
-      </c>
-      <c r="D10" s="1">
-        <v>1.6</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="1">
-        <v>1.4E-2</v>
-      </c>
-      <c r="B11" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0.30599999999999999</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1.48</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1"/>

</xml_diff>